<commit_message>
navigation to accounting module
</commit_message>
<xml_diff>
--- a/Necessary codes/EXCEL/products.xlsx
+++ b/Necessary codes/EXCEL/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karun\PycharmProjects\PythonProject\Necessary codes\EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CF1692-5BCA-455A-B1AE-CA3B4008299C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF8E04E-1A8C-40CA-A5EF-1D2BFC974E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{2ECFD7A8-563D-48F8-9C65-6167ED808DAE}"/>
   </bookViews>
@@ -116,13 +116,13 @@
     <t>WXY</t>
   </si>
   <si>
-    <t>tested 13</t>
-  </si>
-  <si>
-    <t>tested 14</t>
-  </si>
-  <si>
-    <t>tested 15</t>
+    <t>tested 16</t>
+  </si>
+  <si>
+    <t>tested 17</t>
+  </si>
+  <si>
+    <t>tested 188</t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>